<commit_message>
Complétion de l'app streamlit
</commit_message>
<xml_diff>
--- a/Longueurs_Fx.xlsx
+++ b/Longueurs_Fx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,45 +424,30 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>P9</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>P19</t>
+          <t>A17</t>
         </is>
       </c>
       <c r="C1" t="n">
-        <v>2350</v>
+        <v>700</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P9</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A17</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
           <t>A28</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>A30</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C2" t="n">
         <v>570</v>
       </c>
     </row>

</xml_diff>

<commit_message>
path noeuds and graphe maj
</commit_message>
<xml_diff>
--- a/Longueurs_Fx.xlsx
+++ b/Longueurs_Fx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salimelouahdani/Documents/04 - Wiringtek/FaisceauCalc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69791C1-9B19-8842-BCF8-CFAB44063F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB2A639-9D8E-324F-B2D0-746511E4125E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,35 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>A28</t>
+    <t>A30</t>
   </si>
   <si>
-    <t>A30</t>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,14 +74,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{3266FEF0-E844-BA43-A8A2-8A3CA0088D63}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,20 +383,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>